<commit_message>
Interview prep react question added
</commit_message>
<xml_diff>
--- a/Interview Question/Javascript.xlsx
+++ b/Interview Question/Javascript.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vijayanand.Ravi/Personal/EMC/EMC--B17/Interview Question/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vijayanand.Ravi/Personal/EMC/Interview Prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A136B6B-CCEF-A94A-81C5-1C8FF91FD9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B13E53-C33B-254D-9A55-DB5EB3B2FC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="24820" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="760" windowWidth="24840" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="JavaScript" sheetId="7" r:id="rId1"/>
+    <sheet name="Training Plans" sheetId="1" r:id="rId1"/>
+    <sheet name="JavaScript" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,148 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+  <si>
+    <t>Technical Interview Training Workflow</t>
+  </si>
+  <si>
+    <t>Training Session</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Training 1</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Self-introduction </t>
+  </si>
+  <si>
+    <t>15 mins</t>
+  </si>
+  <si>
+    <t>Purpose of the training</t>
+  </si>
+  <si>
+    <t>Explore the training and advantages of enrolling in a Full Stack Development (FSD) course.</t>
+  </si>
+  <si>
+    <t>Softcopy Distribution</t>
+  </si>
+  <si>
+    <t>Inform the students that they will receive a soft copy of key interview questions at the conclusion of each session.</t>
+  </si>
+  <si>
+    <t>End of Session</t>
+  </si>
+  <si>
+    <t>Training 2</t>
+  </si>
+  <si>
+    <t>HTML,CSS and JavaScript Interview Questions</t>
+  </si>
+  <si>
+    <t>Teach important questions and answers from HTML,CSS Advance CSS</t>
+  </si>
+  <si>
+    <t>40 mins</t>
+  </si>
+  <si>
+    <t>Coding Questions</t>
+  </si>
+  <si>
+    <t>Solve coding questions from HTML,CSS Advance CSS</t>
+  </si>
+  <si>
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>Provide softcopy of important interview questions</t>
+  </si>
+  <si>
+    <t>Training 3</t>
+  </si>
+  <si>
+    <t>Review of Previous Session</t>
+  </si>
+  <si>
+    <t>Ask questions from the previous session, give marks</t>
+  </si>
+  <si>
+    <t>30 mins</t>
+  </si>
+  <si>
+    <t>Javascript Questions</t>
+  </si>
+  <si>
+    <t>Teach important questions and answers from Javascript.</t>
+  </si>
+  <si>
+    <t>Solve Javascript coding questions</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>Training 4</t>
+  </si>
+  <si>
+    <t>React Basic Interview Questions</t>
+  </si>
+  <si>
+    <t>Teach important questions and answers from React Hooks, Form Handling Inputs, and Props</t>
+  </si>
+  <si>
+    <t>Teach and solve React Hooks, Form Handling Inputs and Props questions</t>
+  </si>
+  <si>
+    <t>Training 5</t>
+  </si>
+  <si>
+    <t>React Advance Interview Questions</t>
+  </si>
+  <si>
+    <t>Teach important questions and answers from UseContext and REST API Integration, URL Query, Params</t>
+  </si>
+  <si>
+    <t>Solve Usecontext and REST API intergration,URL Query,Params questions</t>
+  </si>
+  <si>
+    <t>Training 6</t>
+  </si>
+  <si>
+    <t>Final Review</t>
+  </si>
+  <si>
+    <t>Review key concepts from all sessions, conduct quiz</t>
+  </si>
+  <si>
+    <t>Node.js, MongoDB, and Express.jsInterview Questions</t>
+  </si>
+  <si>
+    <t>Teach important questions and answers from Node.js, MongoDB, and Express.js</t>
+  </si>
+  <si>
+    <t>Teach and solve Node.js, MongoDB, and Express.js coding questions</t>
+  </si>
+  <si>
+    <t>Closing and Encouragement</t>
+  </si>
+  <si>
+    <t>Summarize key points, encourage students, answer questions, and teach skills needed for full-stack development</t>
+  </si>
+  <si>
+    <t>5 mins</t>
+  </si>
   <si>
     <t>S.No</t>
   </si>
@@ -244,7 +386,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +410,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -280,7 +434,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +455,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF2F75B5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF305496"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -312,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -321,10 +493,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -336,6 +548,89 @@
         <color rgb="FF000000"/>
       </left>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFD9E1F2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD6DCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD6DCE4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD6DCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD6DCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -345,6 +640,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD6DCE4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD6DCE4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -352,6 +684,32 @@
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD6DCE4"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD9E1F2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -376,6 +734,45 @@
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD6DCE4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -459,43 +856,113 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,6 +1298,347 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="43"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="43"/>
+      <c r="B5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="45"/>
+      <c r="B7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="46"/>
+      <c r="B8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="47"/>
+      <c r="B10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="47"/>
+      <c r="B11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="48"/>
+      <c r="B12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="37"/>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="37"/>
+      <c r="B15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
+      <c r="B16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="47"/>
+      <c r="B18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="47"/>
+      <c r="B19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="48"/>
+      <c r="B20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="37"/>
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="37"/>
+      <c r="B23" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="37"/>
+      <c r="B24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
+      <c r="B25" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29819294-9B38-4123-833E-5918D2C3CB39}">
   <dimension ref="C4:E25"/>
   <sheetViews>
@@ -847,238 +1655,238 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="50"/>
+      <c r="E4" s="51"/>
+    </row>
+    <row r="5" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C5" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C6" s="33">
+        <v>1</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C7" s="33">
+        <v>2</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C8" s="33">
         <v>3</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="3:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="D8" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C9" s="33">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="D9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" ht="176" x14ac:dyDescent="0.2">
+      <c r="C10" s="33">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="D10" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C11" s="33">
         <v>6</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="D11" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="C12" s="33">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C8" s="7">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="D12" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="C13" s="33">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="D13" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C14" s="33">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C9" s="7">
-        <v>4</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="D14" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="C15" s="33">
         <v>10</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="D15" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="C16" s="33">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="3:5" ht="176" x14ac:dyDescent="0.2">
-      <c r="C10" s="7">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="D16" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="C17" s="33">
         <v>12</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="D17" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="C18" s="33">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="3:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C11" s="7">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
+      <c r="D18" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="C19" s="33">
         <v>14</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="D19" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="C20" s="33">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="3:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="C12" s="7">
-        <v>7</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="D20" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C21" s="33">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="D21" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="C22" s="33">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="3:5" ht="160" x14ac:dyDescent="0.2">
-      <c r="C13" s="7">
-        <v>8</v>
-      </c>
-      <c r="D13" s="5" t="s">
+      <c r="D22" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C23" s="33">
         <v>18</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="D23" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="C24" s="33">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="3:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C14" s="7">
-        <v>9</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="D24" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="3:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="C25" s="34">
         <v>20</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="3:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="C15" s="7">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="3:5" ht="224" x14ac:dyDescent="0.2">
-      <c r="C16" s="7">
-        <v>11</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" ht="112" x14ac:dyDescent="0.2">
-      <c r="C17" s="7">
-        <v>12</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="144" x14ac:dyDescent="0.2">
-      <c r="C18" s="7">
-        <v>13</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="C19" s="7">
-        <v>14</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" ht="160" x14ac:dyDescent="0.2">
-      <c r="C20" s="7">
-        <v>15</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="C21" s="7">
-        <v>16</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="3:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="C22" s="7">
-        <v>17</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C23" s="7">
-        <v>18</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="C24" s="7">
-        <v>19</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="3:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="C25" s="8">
-        <v>20</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="D25" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>